<commit_message>
Updating to the pre-12 box.
</commit_message>
<xml_diff>
--- a/projects/lhs_docker_example.xlsx
+++ b/projects/lhs_docker_example.xlsx
@@ -2283,7 +2283,7 @@
     <t>3200 GB</t>
   </si>
   <si>
-    <t>2.0.0-pre11</t>
+    <t>2.0.0-pre12</t>
   </si>
 </sst>
 </file>
@@ -5862,7 +5862,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5939,7 +5939,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="28">
       <c r="A7" s="1" t="s">
         <v>441</v>
       </c>

</xml_diff>

<commit_message>
Final changes - increased debugging & tested backwards compatability.
</commit_message>
<xml_diff>
--- a/projects/lhs_docker_example.xlsx
+++ b/projects/lhs_docker_example.xlsx
@@ -2283,7 +2283,7 @@
     <t>3200 GB</t>
   </si>
   <si>
-    <t>2.0.0-pre12</t>
+    <t>2.0.0-pre13</t>
   </si>
 </sst>
 </file>
@@ -5862,7 +5862,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5944,19 +5944,19 @@
         <v>441</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>734</v>
+        <v>591</v>
       </c>
       <c r="C7" s="23" t="str">
         <f>VLOOKUP($B7,instance_defs,5,FALSE)</f>
-        <v>Recommended for Server - Medium Applications</v>
+        <v>Recommended for Server - Small Applications</v>
       </c>
       <c r="D7" s="23" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
-        <v>4 Cores with 800 GB</v>
+        <v>4 Cores with 40 GB</v>
       </c>
       <c r="E7" s="23" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
-        <v>$0.85/hour</v>
+        <v>$0.28/hour</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>605</v>
@@ -5967,7 +5967,7 @@
         <v>442</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>602</v>
+        <v>439</v>
       </c>
       <c r="C8" s="23" t="str">
         <f>VLOOKUP($B8,instance_defs,5,FALSE)</f>
@@ -5975,11 +5975,11 @@
       </c>
       <c r="D8" s="23" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
-        <v>32 Cores with 320 GB</v>
+        <v>8 Cores with 80 GB</v>
       </c>
       <c r="E8" s="23" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
-        <v>$1.68/hour</v>
+        <v>$0.42/hour</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>443</v>
@@ -5990,7 +5990,7 @@
         <v>459</v>
       </c>
       <c r="B9" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$4.21/hour</v>
+        <v>$0.7/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>604</v>

</xml_diff>

<commit_message>
Updating to new AMI V3 json schema.
</commit_message>
<xml_diff>
--- a/projects/lhs_docker_example.xlsx
+++ b/projects/lhs_docker_example.xlsx
@@ -2220,9 +2220,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>triangle</t>
   </si>
   <si>
@@ -2283,7 +2280,10 @@
     <t>3200 GB</t>
   </si>
   <si>
-    <t>2.0.0-pre13</t>
+    <t>2.0.1-rc0</t>
+  </si>
+  <si>
+    <t>dockerized-example</t>
   </si>
 </sst>
 </file>
@@ -5862,7 +5862,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5922,7 +5922,7 @@
         <v>468</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>612</v>
@@ -5933,7 +5933,7 @@
         <v>469</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>726</v>
+        <v>747</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>471</v>
@@ -6692,7 +6692,7 @@
       <c r="P6" s="40"/>
       <c r="Q6" s="40"/>
       <c r="R6" s="39" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="S6" s="39"/>
       <c r="T6" s="39"/>
@@ -7044,7 +7044,7 @@
       <c r="P15" s="40"/>
       <c r="Q15" s="40"/>
       <c r="R15" s="39" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S15" s="39"/>
       <c r="T15" s="39"/>
@@ -7130,7 +7130,7 @@
       <c r="P17" s="39"/>
       <c r="Q17" s="39"/>
       <c r="R17" s="39" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S17" s="39"/>
       <c r="T17" s="39"/>
@@ -7334,7 +7334,7 @@
         <v>719</v>
       </c>
       <c r="R22" s="39" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="S22" s="39"/>
       <c r="T22" s="39"/>
@@ -7534,7 +7534,7 @@
       <c r="P27" s="39"/>
       <c r="Q27" s="39"/>
       <c r="R27" s="39" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="S27" s="39"/>
       <c r="T27" s="39"/>
@@ -7698,7 +7698,7 @@
       <c r="P31" s="39"/>
       <c r="Q31" s="39"/>
       <c r="R31" s="39" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="S31" s="39"/>
       <c r="T31" s="39"/>
@@ -7832,14 +7832,14 @@
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="47" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F35" s="47"/>
       <c r="G35" s="47" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="H35" s="47"/>
       <c r="I35" s="47" t="b">
@@ -7902,7 +7902,7 @@
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
       <c r="R36" s="39" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S36" s="39"/>
       <c r="T36" s="39"/>
@@ -19085,7 +19085,7 @@
         <v>650</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="21" customFormat="1">
@@ -19102,7 +19102,7 @@
         <v>651</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="21" customFormat="1">
@@ -19136,7 +19136,7 @@
         <v>650</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -19192,53 +19192,53 @@
     </row>
     <row r="11" spans="1:7" s="21" customFormat="1">
       <c r="A11" s="21" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>445</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="21" customFormat="1">
       <c r="A12" s="21" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>446</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="21" customFormat="1">
       <c r="A13" s="21" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>447</v>
       </c>
       <c r="C13" s="21" t="s">
+        <v>744</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>745</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>746</v>
-      </c>
       <c r="E13" s="21" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="21" customFormat="1"/>

</xml_diff>